<commit_message>
Finished with everything. Only need to do explanations
</commit_message>
<xml_diff>
--- a/hw2/prob4 pipeline diag.xlsx
+++ b/hw2/prob4 pipeline diag.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="10100" yWindow="480" windowWidth="18700" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="parta" sheetId="1" r:id="rId1"/>
+    <sheet name="partb" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="23">
   <si>
     <t>lw r12, 0(r4)</t>
   </si>
@@ -87,6 +88,12 @@
   </si>
   <si>
     <t>Cycle type:</t>
+  </si>
+  <si>
+    <t>lw r5, 8(r5)</t>
+  </si>
+  <si>
+    <t>lw r4, 4(r4)</t>
   </si>
 </sst>
 </file>
@@ -403,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1128,4 +1135,879 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AP23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AQ1" sqref="AQ1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="52" width="3.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>13</v>
+      </c>
+      <c r="O2">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2">
+        <v>16</v>
+      </c>
+      <c r="R2">
+        <v>17</v>
+      </c>
+      <c r="S2">
+        <v>18</v>
+      </c>
+      <c r="T2">
+        <v>19</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
+      <c r="V2">
+        <v>21</v>
+      </c>
+      <c r="W2">
+        <v>22</v>
+      </c>
+      <c r="X2">
+        <v>23</v>
+      </c>
+      <c r="Y2">
+        <v>24</v>
+      </c>
+      <c r="Z2">
+        <v>25</v>
+      </c>
+      <c r="AA2">
+        <v>26</v>
+      </c>
+      <c r="AB2">
+        <v>27</v>
+      </c>
+      <c r="AC2">
+        <v>28</v>
+      </c>
+      <c r="AD2">
+        <v>29</v>
+      </c>
+      <c r="AE2">
+        <v>30</v>
+      </c>
+      <c r="AF2">
+        <v>31</v>
+      </c>
+      <c r="AG2">
+        <v>32</v>
+      </c>
+      <c r="AH2">
+        <v>33</v>
+      </c>
+      <c r="AI2">
+        <v>34</v>
+      </c>
+      <c r="AJ2">
+        <v>35</v>
+      </c>
+      <c r="AK2">
+        <v>36</v>
+      </c>
+      <c r="AL2">
+        <v>37</v>
+      </c>
+      <c r="AM2">
+        <v>38</v>
+      </c>
+      <c r="AN2">
+        <v>39</v>
+      </c>
+      <c r="AO2">
+        <v>40</v>
+      </c>
+      <c r="AP2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" t="s">
+        <v>9</v>
+      </c>
+      <c r="S8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>7</v>
+      </c>
+      <c r="R9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" t="s">
+        <v>7</v>
+      </c>
+      <c r="S10" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R11" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" t="s">
+        <v>7</v>
+      </c>
+      <c r="T11" t="s">
+        <v>16</v>
+      </c>
+      <c r="U11" t="s">
+        <v>16</v>
+      </c>
+      <c r="V11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12" t="s">
+        <v>6</v>
+      </c>
+      <c r="T12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U12" t="s">
+        <v>16</v>
+      </c>
+      <c r="V12" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>6</v>
+      </c>
+      <c r="U13" t="s">
+        <v>7</v>
+      </c>
+      <c r="V13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W13" t="s">
+        <v>9</v>
+      </c>
+      <c r="X13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
+        <v>6</v>
+      </c>
+      <c r="V14" t="s">
+        <v>7</v>
+      </c>
+      <c r="W14" t="s">
+        <v>8</v>
+      </c>
+      <c r="X14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="V15" t="s">
+        <v>6</v>
+      </c>
+      <c r="W15" t="s">
+        <v>7</v>
+      </c>
+      <c r="X15" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="W16" t="s">
+        <v>6</v>
+      </c>
+      <c r="X16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ18" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>9</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK20" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL23" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM23" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO23" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>